<commit_message>
CR 70 x 60 en DTV
</commit_message>
<xml_diff>
--- a/Fleet Modificaciones solicitadas.xlsx
+++ b/Fleet Modificaciones solicitadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamarin\FleetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8E6FBA-B311-45AE-8BBF-AD3642F6C952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A905E-FF37-499E-8533-2F6314728403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D167E44-E563-4DF9-9CAD-3636B941BCB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Fecha</t>
   </si>
@@ -67,6 +67,30 @@
   </si>
   <si>
     <t>Se corrigió en todos los módulos</t>
+  </si>
+  <si>
+    <t>En la lista de Tasa aparecen algunas OT de una misma persona "duplicadas" (porque  está separando por modelo. Deben salir juntas</t>
+  </si>
+  <si>
+    <t>En DTV agregar botón opción "Otros Recuperos" similar a como es en Tasa</t>
+  </si>
+  <si>
+    <t>V.5 4/1/2022</t>
+  </si>
+  <si>
+    <t>V.2 20/12/2022</t>
+  </si>
+  <si>
+    <t>No pueden cerrar sesión para cambiar de usuario</t>
+  </si>
+  <si>
+    <t>V.4 3/1/2022</t>
+  </si>
+  <si>
+    <t>V.3 29/12/2022</t>
+  </si>
+  <si>
+    <t>En DTV cuando se guarda pone Código cierre 60 y debe ser 70</t>
   </si>
 </sst>
 </file>
@@ -115,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -138,11 +162,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +227,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,11 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4F8DBC-1A7E-4CD8-B2CF-503AC5EB2B70}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C5"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -527,7 +597,9 @@
         <v>44547</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
@@ -542,7 +614,7 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
@@ -557,7 +629,7 @@
       <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -570,39 +642,67 @@
         <v>44547</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="8"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="3"/>
+      <c r="A7" s="3">
+        <v>44564</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8">
+        <v>44564</v>
+      </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8">
+        <v>44565</v>
+      </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8">
+        <v>44565</v>
+      </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3">
+        <v>44565</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -827,15 +927,15 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -859,7 +959,25 @@
       <c r="D46" s="5"/>
       <c r="E46" s="3"/>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E2:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Habilita campo Novedades en el API de Tasa
</commit_message>
<xml_diff>
--- a/Fleet Modificaciones solicitadas.xlsx
+++ b/Fleet Modificaciones solicitadas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamarin\FleetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A905E-FF37-499E-8533-2F6314728403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC360DC8-CF0E-4042-B229-C7CE7B293A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D167E44-E563-4DF9-9CAD-3636B941BCB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Fecha</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>En DTV cuando se guarda pone Código cierre 60 y debe ser 70</t>
+  </si>
+  <si>
+    <t>V.6 5/1/2022</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -703,9 +706,13 @@
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="8">
+        <v>44566</v>
+      </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>

</xml_diff>

<commit_message>
Cambios en el API de los graficos
</commit_message>
<xml_diff>
--- a/Fleet Modificaciones solicitadas.xlsx
+++ b/Fleet Modificaciones solicitadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Xamarin\FleetApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC360DC8-CF0E-4042-B229-C7CE7B293A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AC5374-AC0E-4772-9775-43141C759466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D167E44-E563-4DF9-9CAD-3636B941BCB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Fecha</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>V.6 5/1/2022</t>
+  </si>
+  <si>
+    <t>Que se vea el campo Novedades en las Obras de Tasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cambio en API</t>
   </si>
 </sst>
 </file>
@@ -559,7 +565,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -715,11 +721,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
+      <c r="A11" s="3">
+        <v>44578</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="8">
+        <v>44578</v>
+      </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>

</xml_diff>